<commit_message>
intégration balise sémantique + balise content
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99318D81-283F-074B-B660-D82EADF451FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4D6E9E-9EB8-6E42-A9A5-3CB21B0FEE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="460" windowWidth="27860" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Catégorie</t>
   </si>
@@ -70,13 +70,51 @@
   </si>
   <si>
     <t>balise html "title"</t>
+  </si>
+  <si>
+    <t>la balise title est une balise très importante étant donné que c'est elle qui va initier le sujet principal de la page et un point n'explique en rien le but ou sujet de la page</t>
+  </si>
+  <si>
+    <t>Optimisez le contenu de vos pages</t>
+  </si>
+  <si>
+    <t>Mettre dans cette balise le mot clé le plus important pour traiter du sujet de la page. 
+Exemple  : &lt;title&gt;La Chouette Agence - Entreprise de web design basé sur Lyon&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t>balise meta description
+ et content</t>
+  </si>
+  <si>
+    <t>Accessibilité/ Seo</t>
+  </si>
+  <si>
+    <t>absence balise sémantique html</t>
+  </si>
+  <si>
+    <t>Balise sémantique et SEO</t>
+  </si>
+  <si>
+    <t>Utiliser les balises sémantiques tel que main, section, article, footer etc 
+pour mieux découper le html</t>
+  </si>
+  <si>
+    <t>Les balises sémantiques sont plus pertinente niveau accessibilité des contenu pour les personnes qui utilisent des logiciels de lecture de site web</t>
+  </si>
+  <si>
+    <t>La balise description aide Google à savoir de quoi parlent la page, 
+et c’est aussi ce qui est affiché sous title dans les résultats de recherchent, ce qui permet aux utilisateurs de savoir de quoi traite le site</t>
+  </si>
+  <si>
+    <t>Faire une description précise du sujet de la page.
+Remplacer la description par : "La Chouette Agence est une entreprise de webdesign basé à Lyon qui aide les entreprises a développer leur image et leur branding sur le Web» serait plus pertinent.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,6 +151,19 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -148,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,6 +208,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -375,14 +434,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" customWidth="1"/>
+    <col min="3" max="3" width="129.7109375" customWidth="1"/>
     <col min="4" max="4" width="64" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="57" customWidth="1"/>
@@ -436,7 +495,7 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -449,20 +508,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="4"/>
+    <row r="4" spans="1:26" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="4"/>
+    <row r="5" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="4"/>
@@ -1482,6 +1586,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{8AC3B716-3A86-9E43-8D5C-688C285B70CF}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{5A6CC508-8734-E74B-A9A6-A86E08F4DE91}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{D50E4972-5D37-4E45-AFA7-F9D9B94DF4C7}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{077AF545-4964-6045-9DF4-92AFE5E34377}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
augmentation taille police texte
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4D6E9E-9EB8-6E42-A9A5-3CB21B0FEE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A531C9A-2257-E945-8E6F-185CA06563F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="27860" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="680" windowWidth="25140" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Catégorie</t>
   </si>
@@ -108,6 +108,38 @@
   <si>
     <t>Faire une description précise du sujet de la page.
 Remplacer la description par : "La Chouette Agence est une entreprise de webdesign basé à Lyon qui aide les entreprises a développer leur image et leur branding sur le Web» serait plus pertinent.</t>
+  </si>
+  <si>
+    <t>Amélioration technique</t>
+  </si>
+  <si>
+    <t>Format des images
+trop lourd</t>
+  </si>
+  <si>
+    <t>Les images au format JPG ou PNG ne sont pas les plus adaptés niveau SEO étant donné que la page met plus de temps à charger.</t>
+  </si>
+  <si>
+    <t>Les formats d'image tel WebP proposent souvent une meilleure compression que les formats PNG ou JPEG. Ce qui fait que le téléchargements des images est plus rapides, amenant une consommation de données réduite pour une page qui charge plus vite</t>
+  </si>
+  <si>
+    <t>anthedesign.fr</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Texte dans une taile trop petite</t>
+  </si>
+  <si>
+    <t>Un texte trop petit peut être génant pour les utilisateurs ; ils devront faire des efforts pour lire 
+Cela est d'autant plus problématique pour les personnes aillant des problèmes lié à la vue</t>
+  </si>
+  <si>
+    <t>www.affde.com</t>
+  </si>
+  <si>
+    <t>Augmenter la taille du texte serait confortable pour les utilisateurs du site, les amenant à faire moins d'effort. C'est aussi un plus pour le côté responsive sur mobile</t>
   </si>
 </sst>
 </file>
@@ -434,13 +466,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="129.7109375" customWidth="1"/>
     <col min="4" max="4" width="64" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
@@ -568,11 +601,45 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E6" s="4"/>
+    <row r="6" spans="1:26" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E7" s="4"/>
+    <row r="7" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E8" s="4"/>
@@ -1589,6 +1656,8 @@
     <hyperlink ref="F3" r:id="rId2" xr:uid="{5A6CC508-8734-E74B-A9A6-A86E08F4DE91}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{D50E4972-5D37-4E45-AFA7-F9D9B94DF4C7}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{077AF545-4964-6045-9DF4-92AFE5E34377}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{C1A96893-84DB-9341-8D9E-C0DB81588B50}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{E7D94CD9-65E2-184D-9BDC-D9FB3E0C13B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
mise à jour fichier audit
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A531C9A-2257-E945-8E6F-185CA06563F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECB3852-090D-194C-B898-DE6A3829DC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="680" windowWidth="25140" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Catégorie</t>
   </si>
@@ -140,6 +140,20 @@
   </si>
   <si>
     <t>Augmenter la taille du texte serait confortable pour les utilisateurs du site, les amenant à faire moins d'effort. C'est aussi un plus pour le côté responsive sur mobile</t>
+  </si>
+  <si>
+    <t>Mots clés en petit sur fond blanc</t>
+  </si>
+  <si>
+    <t>Les div avec la classe "keywords" contient une succession de mots clés sans contexte. 
+Il s’agit d’une technique de "triche" pour booster frauduleusement son référencement.</t>
+  </si>
+  <si>
+    <t>Essayer de tromper l'algorithme de Google représente un risque pour le référencement de la page car cela pourrait entrainer un malus.
+Suppression de ces divs là où elles apparaissent (header + footer)</t>
+  </si>
+  <si>
+    <t>smartkeyword - Black Hat</t>
   </si>
 </sst>
 </file>
@@ -466,14 +480,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="129.7109375" customWidth="1"/>
     <col min="4" max="4" width="64" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
@@ -641,8 +655,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E8" s="4"/>
+    <row r="8" spans="1:26" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="4"/>
@@ -1658,6 +1689,7 @@
     <hyperlink ref="F5" r:id="rId4" xr:uid="{077AF545-4964-6045-9DF4-92AFE5E34377}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{C1A96893-84DB-9341-8D9E-C0DB81588B50}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{E7D94CD9-65E2-184D-9BDC-D9FB3E0C13B1}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{06C416C1-F608-1140-9B28-509633383B8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
mise à jour audit Excell
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E6525-A4ED-7944-A917-691C243CAB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44325A8E-91A7-194E-B7BB-87FCDA82E8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="680" windowWidth="25140" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Catégorie</t>
   </si>
@@ -145,15 +145,30 @@
     <t>Mots clés en petit sur fond blanc</t>
   </si>
   <si>
-    <t>Les div avec la classe "keywords" contient une succession de mots clés sans contexte. 
+    <t>smartkeyword - Black Hat</t>
+  </si>
+  <si>
+    <t>Les div avec la classe "keywords" contient une succession de mots clés sans contexte pour tromper l'algo' Google, c'est une technique de blackhat.
 Il s’agit d’une technique de "triche" pour booster frauduleusement son référencement.</t>
   </si>
   <si>
     <t>Essayer de tromper l'algorithme de Google représente un risque pour le référencement de la page car cela pourrait entrainer un malus.
-Suppression de ces divs là où elles apparaissent (header + footer)</t>
-  </si>
-  <si>
-    <t>smartkeyword - Black Hat</t>
+Suppression de ces divs là où elles apparaissent (header + footer donc)</t>
+  </si>
+  <si>
+    <t>SEO et Accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balises Alt </t>
+  </si>
+  <si>
+    <t>La balises html Alt est certaines fois absente, mais quand elle est présente les mots cités ne décrivent pas le contenu de l'image. Cette balises est très utile pour les malvoyants mais aussi pour Google.</t>
+  </si>
+  <si>
+    <t>Ajout de la balise Alt sur les images qui ne l’ont pas et modification de leur contenu par des descriptions justes et concises.</t>
+  </si>
+  <si>
+    <t>smartkeyword - Alt</t>
   </si>
 </sst>
 </file>
@@ -480,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -663,20 +678,37 @@
         <v>34</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E10" s="4"/>
@@ -1690,6 +1722,7 @@
     <hyperlink ref="F6" r:id="rId5" xr:uid="{C1A96893-84DB-9341-8D9E-C0DB81588B50}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{E7D94CD9-65E2-184D-9BDC-D9FB3E0C13B1}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{06C416C1-F608-1140-9B28-509633383B8F}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{85B269BF-C3E1-5F4C-A6EC-8D2CFFEB3794}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
correction du titre H1
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44325A8E-91A7-194E-B7BB-87FCDA82E8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFFF235-BB47-314D-AC95-0125C79F10EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="680" windowWidth="25140" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="25140" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Catégorie</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>smartkeyword - Alt</t>
+  </si>
+  <si>
+    <t>Titre H1</t>
+  </si>
+  <si>
+    <t>La balise H1 contient seulement les mots "La chouette agence." Il faudrait mettre plus de mots pertinent pour plus d'efficacité.</t>
+  </si>
+  <si>
+    <t>smartkeyword - Balise H1</t>
+  </si>
+  <si>
+    <t>Le titre H1 doit contenir des mots clés qui décrivent correctement le site comme par exemple "La Chouette Agence – Entreprise de webdesign basé à Lyon"</t>
   </si>
 </sst>
 </file>
@@ -495,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -710,8 +722,25 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:26" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E11" s="4"/>
@@ -1723,6 +1752,7 @@
     <hyperlink ref="F7" r:id="rId6" xr:uid="{E7D94CD9-65E2-184D-9BDC-D9FB3E0C13B1}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{06C416C1-F608-1140-9B28-509633383B8F}"/>
     <hyperlink ref="F9" r:id="rId8" xr:uid="{85B269BF-C3E1-5F4C-A6EC-8D2CFFEB3794}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{C2BE3E34-6520-2647-8D11-348C608196FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
mise à jour et finition fichier Excell
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2087F1F-B883-0440-9841-1ADD5FCFE085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32185C8F-CAB2-2D42-BF3F-B5928993D59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="25140" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>Catégorie</t>
   </si>
@@ -224,6 +224,67 @@
   </si>
   <si>
     <t>Bouton "Contactez notre équipe" agrandi pour le tactile</t>
+  </si>
+  <si>
+    <t>Oubli des attributs defer sur les scripts JS</t>
+  </si>
+  <si>
+    <t>Sans l’attribut defer, les scripts JS chargent en même temps que le CSS/HTML, pouvant ralentir le chargement du site</t>
+  </si>
+  <si>
+    <t>Rajout de l'attribut defer sur tout les scripts JS</t>
+  </si>
+  <si>
+    <t>oncrawl</t>
+  </si>
+  <si>
+    <t>Script JS en début de page</t>
+  </si>
+  <si>
+    <t>Les différents scripts JS sont placé au niveau du head, entrainant un temps de chargement supplémentaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placer les scripts à la fin du HTML avant la balise de fermeture du body.
+Il ne chargera donc pas dés le début </t>
+  </si>
+  <si>
+    <t>CSS non minifié</t>
+  </si>
+  <si>
+    <t>Un fichier CSS qui n'est pas minifié mettra plus de temps à charger, ralentissant ainsi la vitesse de chargement du site et par la même occasion ses performances techniques.</t>
+  </si>
+  <si>
+    <t>Minifier le CSS</t>
+  </si>
+  <si>
+    <t>dareboost - La Minification CSS</t>
+  </si>
+  <si>
+    <t>Menu, formulaire etc sur page 2</t>
+  </si>
+  <si>
+    <t>Le menu est quasiment entièrement au bord de la fenêtre ce qui fait qu'il est considéré comme caché et le contenu caché est pénalisé par Google. 
+Le formulaire est aussi mal intégré, tout ça réunit fait que la navigation n'est pas des plus optimales.</t>
+  </si>
+  <si>
+    <t>Appliquer le même fichier CSS au deux pages pour unifier l'affichage</t>
+  </si>
+  <si>
+    <t>la page de contact porte un mauvais nom</t>
+  </si>
+  <si>
+    <t>Le nom de la page pour contacter La Chouette Agence est « page2 ». Ce n'est pas le plus optimale pour l'algo' de Google.</t>
+  </si>
+  <si>
+    <t>Changer le nom de cette page en quelque chose de beaucoup plus explicite
+ comme contact.html pour qu'elle sois plus facilement localisable sur les résultats 
+de recherche et ainsi éviter qu'elle sois difficile à trouver par des internautes</t>
+  </si>
+  <si>
+    <t>smartkeyword</t>
+  </si>
+  <si>
+    <t>josselinleydier</t>
   </si>
 </sst>
 </file>
@@ -427,13 +488,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -482,23 +538,59 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -719,333 +811,411 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="129.7109375" customWidth="1"/>
-    <col min="4" max="4" width="64" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="57" customWidth="1"/>
-    <col min="7" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="12" width="0.140625" customWidth="1"/>
-    <col min="13" max="15" width="10.5703125" customWidth="1"/>
-    <col min="16" max="16" width="127" customWidth="1"/>
-    <col min="17" max="26" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="135.42578125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="64" style="25" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="57" style="25" customWidth="1"/>
+    <col min="7" max="8" width="10.5703125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="10" style="25" customWidth="1"/>
+    <col min="10" max="12" width="0.140625" style="25" customWidth="1"/>
+    <col min="13" max="15" width="10.5703125" style="25" customWidth="1"/>
+    <col min="16" max="16" width="127" style="25" customWidth="1"/>
+    <col min="17" max="26" width="10.5703125" style="25" customWidth="1"/>
+    <col min="27" max="16384" width="11.28515625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
     </row>
     <row r="2" spans="1:26" ht="22" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:26" ht="61" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="23" t="s">
+      <c r="P3" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="102" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="39" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="25"/>
+      <c r="P5" s="21"/>
     </row>
     <row r="6" spans="1:26" ht="64" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O6" s="22" t="s">
+      <c r="O6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="P6" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="51" customHeight="1">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="O7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="24"/>
+      <c r="P7" s="20"/>
     </row>
     <row r="8" spans="1:26" ht="52" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="36" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="71" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E12" s="3"/>
+    <row r="12" spans="1:26" ht="22" customHeight="1">
+      <c r="A12" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="27" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E13" s="3"/>
+    <row r="13" spans="1:26" ht="38" customHeight="1">
+      <c r="A13" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="27" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E14" s="3"/>
+    <row r="14" spans="1:26" ht="28" customHeight="1">
+      <c r="A14" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="27" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E15" s="3"/>
+    <row r="15" spans="1:26" ht="36" customHeight="1">
+      <c r="A15" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="34" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="52" customHeight="1">
+      <c r="A16" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="F16" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2052,6 +2222,11 @@
     <hyperlink ref="N6" r:id="rId14" location="les_équivalents_textuels" xr:uid="{F8A9C2AE-9B6C-0B4C-8DE9-BB2163AB0459}"/>
     <hyperlink ref="N7" r:id="rId15" location="la_gestion_des_états" xr:uid="{EB0F0208-4AB8-DF4B-B41A-63EA88F0ADF8}"/>
     <hyperlink ref="N8" r:id="rId16" location="principales_recommandations" xr:uid="{3E34818C-A405-9B4C-BFB1-0B71D8245A2D}"/>
+    <hyperlink ref="F12" r:id="rId17" xr:uid="{511EFF83-1E62-0E4D-B27D-A1BEC0A3A5BE}"/>
+    <hyperlink ref="F13" r:id="rId18" xr:uid="{A83E2B72-E54E-AB42-A2E2-2878FFE9FD1C}"/>
+    <hyperlink ref="F14" r:id="rId19" xr:uid="{E0A26AD6-9696-8141-8F35-E6074D8D5010}"/>
+    <hyperlink ref="F16" r:id="rId20" xr:uid="{DF7A1C1E-ACDD-9E47-8115-A86421FB67A7}"/>
+    <hyperlink ref="F15" r:id="rId21" xr:uid="{03BFA441-CA51-B047-8A3F-4D6F8F04DC6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
création page "contactez support" et supp' page 2
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32185C8F-CAB2-2D42-BF3F-B5928993D59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E361AE8-AEA1-5F44-B925-81633338A1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,15 +276,15 @@
     <t>Le nom de la page pour contacter La Chouette Agence est « page2 ». Ce n'est pas le plus optimale pour l'algo' de Google.</t>
   </si>
   <si>
+    <t>smartkeyword</t>
+  </si>
+  <si>
+    <t>josselinleydier</t>
+  </si>
+  <si>
     <t>Changer le nom de cette page en quelque chose de beaucoup plus explicite
- comme contact.html pour qu'elle sois plus facilement localisable sur les résultats 
+ comme "Contactez le support" pour qu'elle sois plus facilement localisable sur les résultats 
 de recherche et ainsi éviter qu'elle sois difficile à trouver par des internautes</t>
-  </si>
-  <si>
-    <t>smartkeyword</t>
-  </si>
-  <si>
-    <t>josselinleydier</t>
   </si>
 </sst>
 </file>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1195,10 +1195,10 @@
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="52" customHeight="1">
+    <row r="16" spans="1:26" ht="82" customHeight="1">
       <c r="A16" s="31" t="s">
         <v>6</v>
       </c>
@@ -1209,11 +1209,11 @@
         <v>76</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
mise à jour fichier audit et correction page2
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E361AE8-AEA1-5F44-B925-81633338A1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E5541-09C2-914B-B185-43590399165B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1106,7 +1106,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+    <row r="11" spans="1:26" ht="27" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
mise à jour audit
</commit_message>
<xml_diff>
--- a/seo /Modèle-audit-SEO.xlsx
+++ b/seo /Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anaschoukri/Documents/Document formation Open Classrooms/Projet 4/seo /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E5541-09C2-914B-B185-43590399165B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D52A4E-62B4-8940-984B-DFA627B55FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1099,9 +1099,7 @@
       <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="4" t="s">
         <v>43</v>
       </c>
@@ -1119,9 +1117,7 @@
       <c r="D11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1139,7 +1135,9 @@
       <c r="D12" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="F12" s="27" t="s">
         <v>64</v>
       </c>
@@ -1211,7 +1209,9 @@
       <c r="D16" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="31" t="s">
+        <v>9</v>
+      </c>
       <c r="F16" s="33" t="s">
         <v>77</v>
       </c>

</xml_diff>